<commit_message>
changes to S-48-100_xyz - images&translations correction
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/connectors.en.xlsx
+++ b/docs/Manual/source/tab/connectors.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="59"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="60"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="531">
   <si>
     <t xml:space="preserve">This is a workbook with source tables of TGZ/TGS connector descriptions in English. Each sheet corresponds to one unique connector type. Since connectors are often repeated within TGZ (typically those on the control board), they are only listed once. I.e. E.g. IO connector 22pin weidmuller B2CF is used over and over again, so it is only listed here once as "X8_IO_22pin_B2CF"</t>
   </si>
@@ -1685,10 +1685,13 @@
     <t xml:space="preserve">brake resistor overtemperature</t>
   </si>
   <si>
+    <t xml:space="preserve">permanently on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCbus undervoltage + mains error. Softstart disabled. No other errors.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Green LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permanently on</t>
   </si>
   <si>
     <t xml:space="preserve">device ready, no errors</t>
@@ -1719,11 +1722,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="0000"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0000"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1844,7 +1846,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1864,7 +1866,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1872,7 +1874,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2057,7 +2059,7 @@
             <v>#X10_CAN_4pin_B2CF</v>
           </cell>
           <cell r="B4" t="str">
-            <v>B2CF 3.50/04/180 SN OR BX</v>
+            <v>B2CF 3.50/04/180 SN OR BX </v>
           </cell>
           <cell r="C4" t="str">
             <v>Weidmüller</v>
@@ -2071,7 +2073,7 @@
             <v>#X6_FB1_8pin_B2CF</v>
           </cell>
           <cell r="B5" t="str">
-            <v>B2CF 3.50/08/180 SN OR BX</v>
+            <v>B2CF 3.50/08/180 SN OR BX </v>
           </cell>
           <cell r="C5" t="str">
             <v>Weidmüller</v>
@@ -2085,7 +2087,7 @@
             <v>#X7_FB2_8pin_B2CF</v>
           </cell>
           <cell r="B6" t="str">
-            <v>B2CF 3.50/08/180 SN OR BX</v>
+            <v>B2CF 3.50/08/180 SN OR BX </v>
           </cell>
           <cell r="C6" t="str">
             <v>Weidmüller</v>
@@ -2099,7 +2101,7 @@
             <v>#X5_FBE_12pin_B2CF</v>
           </cell>
           <cell r="B7" t="str">
-            <v>B2CF 3.50/12/180 SN OR BX</v>
+            <v>B2CF 3.50/12/180 SN OR BX </v>
           </cell>
           <cell r="C7" t="str">
             <v>Weidmüller</v>
@@ -2113,7 +2115,7 @@
             <v>#X1_24V_5pin_BCZ</v>
           </cell>
           <cell r="B8" t="str">
-            <v>BCZ 3.81/05/180 SN OR BX</v>
+            <v>BCZ 3.81/05/180 SN OR BX </v>
           </cell>
           <cell r="C8" t="str">
             <v>Weidmüller</v>
@@ -2127,7 +2129,7 @@
             <v>#X3_M1_6pin_BLZP</v>
           </cell>
           <cell r="B9" t="str">
-            <v>BLZP 5.08HC/06/180 SN OR BX</v>
+            <v>BLZP 5.08HC/06/180 SN OR BX </v>
           </cell>
           <cell r="C9" t="str">
             <v>Weidmüller</v>
@@ -2141,7 +2143,7 @@
             <v>#X4_M2_6pin_BLZP</v>
           </cell>
           <cell r="B10" t="str">
-            <v>BLZP 5.08HC/06/180 SN OR BX</v>
+            <v>BLZP 5.08HC/06/180 SN OR BX </v>
           </cell>
           <cell r="C10" t="str">
             <v>Weidmüller</v>
@@ -2155,7 +2157,7 @@
             <v>#X2_48_DC_1778065</v>
           </cell>
           <cell r="B11" t="str">
-            <v>PC 5/ 2-STCL1-7,62</v>
+            <v>PC 5/ 2-STCL1-7,62 </v>
           </cell>
           <cell r="C11" t="str">
             <v>Phoenix Contact</v>
@@ -2169,7 +2171,7 @@
             <v>#X4_M1_6pin_SLS</v>
           </cell>
           <cell r="B12" t="str">
-            <v>SLS 5.08/06/180FI SN OR BX</v>
+            <v>SLS 5.08/06/180FI SN OR BX </v>
           </cell>
           <cell r="C12" t="str">
             <v>Weidmüller</v>
@@ -2183,7 +2185,7 @@
             <v>#X2_PWR_10pin_BLZP</v>
           </cell>
           <cell r="B13" t="str">
-            <v>BLZP 5.08HC/10/180 SN OR BX</v>
+            <v>BLZP 5.08HC/10/180 SN OR BX </v>
           </cell>
           <cell r="C13" t="str">
             <v>Weidmüller</v>
@@ -2197,7 +2199,7 @@
             <v>#X4_M1_6pin_BLF</v>
           </cell>
           <cell r="B14" t="str">
-            <v>BLF 7.62HP/06/180F</v>
+            <v>BLF 7.62HP/06/180F </v>
           </cell>
           <cell r="C14" t="str">
             <v>Weidmüller</v>
@@ -2211,7 +2213,7 @@
             <v>#X2_PWR_12pin_BLZ</v>
           </cell>
           <cell r="B15" t="str">
-            <v>BLZ 7.62HP/12/180F</v>
+            <v>BLZ 7.62HP/12/180F </v>
           </cell>
           <cell r="C15" t="str">
             <v>Weidmüller</v>
@@ -2225,7 +2227,7 @@
             <v>#X3_M1_4pin_wago_2636</v>
           </cell>
           <cell r="B16" t="str">
-            <v>PC 5/ 2-STCL1-7,62</v>
+            <v>PC 5/ 2-STCL1-7,62 </v>
           </cell>
           <cell r="C16" t="str">
             <v>Phoenix Contact</v>
@@ -2239,7 +2241,7 @@
             <v>#X4_M2_4pin_wago_2636</v>
           </cell>
           <cell r="B17" t="str">
-            <v>PC 5/ 2-STCL1-7,62</v>
+            <v>PC 5/ 2-STCL1-7,62 </v>
           </cell>
           <cell r="C17" t="str">
             <v>Phoenix Contact</v>
@@ -2295,7 +2297,7 @@
             <v>#X1_ACIN_PC5</v>
           </cell>
           <cell r="B21" t="str">
-            <v>PC 5/ 8-STCL1-7,62</v>
+            <v>PC 5/ 8-STCL1-7,62 </v>
           </cell>
           <cell r="C21" t="str">
             <v>Phoenix Contact</v>
@@ -2309,7 +2311,7 @@
             <v>#X2_DC_8pin_PC5</v>
           </cell>
           <cell r="B22" t="str">
-            <v>PC 5/ 8-STCL1-7,62</v>
+            <v>PC 5/ 8-STCL1-7,62 </v>
           </cell>
           <cell r="C22" t="str">
             <v>Phoenix Contact</v>
@@ -2323,7 +2325,7 @@
             <v>#X3_DO_4pin_BCZ</v>
           </cell>
           <cell r="B23" t="str">
-            <v>BCZ 3.81/04/180 SN BK BX</v>
+            <v>BCZ 3.81/04/180 SN BK BX </v>
           </cell>
           <cell r="C23" t="str">
             <v>Weidmüller</v>
@@ -2337,7 +2339,7 @@
             <v>#X3_24V_BLF_2_5</v>
           </cell>
           <cell r="B24" t="str">
-            <v>BLF 2.50/04/180 SN OR BX</v>
+            <v>BLF 2.50/04/180 SN OR BX </v>
           </cell>
           <cell r="C24" t="str">
             <v>Weidmüller</v>
@@ -2351,7 +2353,7 @@
             <v>#X10_CAN_4pin_B2CF</v>
           </cell>
           <cell r="B25" t="str">
-            <v>BCZ 3.81/04/180 SN OR BX</v>
+            <v>BCZ 3.81/04/180 SN OR BX </v>
           </cell>
           <cell r="C25" t="str">
             <v>Weidmüller</v>
@@ -2365,7 +2367,7 @@
             <v>#X5_DI_10pin_B2CF</v>
           </cell>
           <cell r="B26" t="str">
-            <v>B2CF 3.50/10/180 SN OR BX</v>
+            <v>B2CF 3.50/10/180 SN OR BX </v>
           </cell>
           <cell r="C26" t="str">
             <v>Weidmüller</v>
@@ -2379,7 +2381,7 @@
             <v>#X10_DO_10pin_B2CF</v>
           </cell>
           <cell r="B27" t="str">
-            <v>B2CF 3.50/10/180 SN OR BX</v>
+            <v>B2CF 3.50/10/180 SN OR BX </v>
           </cell>
           <cell r="C27" t="str">
             <v>Weidmüller</v>
@@ -2393,7 +2395,7 @@
             <v>#X1_24V_5pin_BCZ_TGM</v>
           </cell>
           <cell r="B28" t="str">
-            <v>BCZ 3.81/05/180 SN OR BX</v>
+            <v>BCZ 3.81/05/180 SN OR BX </v>
           </cell>
           <cell r="C28" t="str">
             <v>Weidmüller</v>
@@ -2407,7 +2409,7 @@
             <v>#X2_320_DC_1778078</v>
           </cell>
           <cell r="B29" t="str">
-            <v>PC 5/ 3-STCL1-7,62</v>
+            <v>PC 5/ 3-STCL1-7,62 </v>
           </cell>
           <cell r="C29" t="str">
             <v>Phoenix Contact</v>
@@ -2421,7 +2423,7 @@
             <v>#X6_FB1_8pin_B2CF_TGM</v>
           </cell>
           <cell r="B30" t="str">
-            <v>BCZ 3.81/08/180 SN OR BX</v>
+            <v>BCZ 3.81/08/180 SN OR BX </v>
           </cell>
           <cell r="C30" t="str">
             <v>Weidmüller</v>
@@ -2435,7 +2437,7 @@
             <v>#X7_FB2_8pin_B2CF_TGM</v>
           </cell>
           <cell r="B31" t="str">
-            <v>BCZ 3.81/08/180 SN OR BX</v>
+            <v>BCZ 3.81/08/180 SN OR BX </v>
           </cell>
           <cell r="C31" t="str">
             <v>Weidmüller</v>
@@ -2449,7 +2451,7 @@
             <v>#X5_FBE_12pin_B2CF_TGM</v>
           </cell>
           <cell r="B32" t="str">
-            <v>BCZ 3.81/12/180 SN OR BX</v>
+            <v>BCZ 3.81/12/180 SN OR BX </v>
           </cell>
           <cell r="C32" t="str">
             <v>Weidmüller</v>
@@ -2575,7 +2577,7 @@
             <v>#X2_560_DC_3pin_BLZ__7_62</v>
           </cell>
           <cell r="B41" t="str">
-            <v>BLZ 7.62HP/03/180LR SN BK BX</v>
+            <v>BLZ 7.62HP/03/180LR SN BK BX </v>
           </cell>
           <cell r="C41" t="str">
             <v>Weidmüller</v>
@@ -2589,7 +2591,7 @@
             <v>#X4_ACIN_4pin_TGS560_25</v>
           </cell>
           <cell r="B42" t="str">
-            <v>BVZ 7.62HP/04/180F SN BK BX</v>
+            <v>BVZ 7.62HP/04/180F SN BK BX </v>
           </cell>
           <cell r="C42" t="str">
             <v>Weidmüller</v>
@@ -2603,7 +2605,7 @@
             <v>#X1_DC_6pin_TGS560_25</v>
           </cell>
           <cell r="B43" t="str">
-            <v>BVZ 7.62HP/06/180F SN BK BX</v>
+            <v>BVZ 7.62HP/06/180F SN BK BX </v>
           </cell>
           <cell r="C43" t="str">
             <v>Weidmüller</v>
@@ -2617,7 +2619,7 @@
             <v>#X5_RBR_3pin_TGS560_25</v>
           </cell>
           <cell r="B44" t="str">
-            <v>BLZ 7.62HP/03/180F SN BK BX</v>
+            <v>BLZ 7.62HP/03/180F SN BK BX </v>
           </cell>
           <cell r="C44" t="str">
             <v>Weidmüller</v>
@@ -2631,7 +2633,7 @@
             <v>#S1_TGS560_DIP</v>
           </cell>
           <cell r="B45" t="str">
-            <v>DS03-254-04BE</v>
+            <v>DS03-254-04BE </v>
           </cell>
           <cell r="C45" t="str">
             <v>Same Sky</v>
@@ -2645,7 +2647,7 @@
             <v>#X4_TGS560_24V_5pin_BCZ</v>
           </cell>
           <cell r="B46" t="str">
-            <v>BCZ 3.81/05/180F SN OR BX</v>
+            <v>BCZ 3.81/05/180F SN OR BX </v>
           </cell>
           <cell r="C46" t="str">
             <v>Weidmüller</v>
@@ -2687,7 +2689,7 @@
             <v>#XBR_BR_6pin_BLF</v>
           </cell>
           <cell r="B49" t="str">
-            <v>BLF 5.00HC/06/180F SN OR BX          </v>
+            <v>BLF 5.00HC/06/180F SN OR BX           </v>
           </cell>
           <cell r="C49" t="str">
             <v>Weidmüller</v>
@@ -18324,7 +18326,7 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -18576,10 +18578,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18696,41 +18698,50 @@
       <c r="I9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="13"/>
+      <c r="A10" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A11" s="13"/>
       <c r="I11" s="14"/>
       <c r="J11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>522</v>
+        <v>134</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>523</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>524</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>525</v>
+      </c>
       <c r="I14" s="14"/>
       <c r="J14" s="13"/>
     </row>
@@ -18755,12 +18766,16 @@
       <c r="J19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13"/>
       <c r="I20" s="14"/>
       <c r="J20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -18816,7 +18831,7 @@
         <v>467</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18830,7 +18845,7 @@
         <v>301</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18844,7 +18859,7 @@
         <v>303</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18858,7 +18873,7 @@
         <v>305</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18927,10 +18942,10 @@
         <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18941,10 +18956,10 @@
         <v>148</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18958,7 +18973,7 @@
         <v>467</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18969,10 +18984,10 @@
         <v>146</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18983,10 +18998,10 @@
         <v>148</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19000,7 +19015,7 @@
         <v>467</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19066,7 +19081,7 @@
         <v>307</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19077,10 +19092,10 @@
         <v>308</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19094,7 +19109,7 @@
         <v>464</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
TGS-560-50_100 connectors renamed according to other standards
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/connectors.en.xlsx
+++ b/docs/Manual/source/tab/connectors.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="56"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -45,7 +45,7 @@
     <sheet name="X15_BR2_4pin_LSF" sheetId="35" state="visible" r:id="rId37"/>
     <sheet name="X1_ACIN_PC5" sheetId="36" state="visible" r:id="rId38"/>
     <sheet name="X2_DC_8pin_PC5" sheetId="37" state="visible" r:id="rId39"/>
-    <sheet name="X3_DO_4pin_BCZ" sheetId="38" state="visible" r:id="rId40"/>
+    <sheet name="X2_DO_4pin_BCZ" sheetId="38" state="visible" r:id="rId40"/>
     <sheet name="X3_24V_BLF_2_5" sheetId="39" state="visible" r:id="rId41"/>
     <sheet name="X5_DI_10pin_B2CF" sheetId="40" state="visible" r:id="rId42"/>
     <sheet name="X10_DO_10pin_B2CF" sheetId="41" state="visible" r:id="rId43"/>
@@ -2077,13 +2077,13 @@
       <sheetName val="X10_CAN_8pin_ClikMate"/>
       <sheetName val="X11_FB3_10pin_ClikMate"/>
       <sheetName val="X12_UDP_8pin_ClikMate"/>
-      <sheetName val="X2_ACIN_7pin_2636"/>
-      <sheetName val="X6_TGS560_50_DCbus"/>
-      <sheetName val="X4_TGS560_24V_5pin_BCZ"/>
+      <sheetName val="X1_ACIN_7pin_2636"/>
+      <sheetName val="X4_TGS560_50_DCbus"/>
+      <sheetName val="X3_TGS560_24V_5pin_BCZ"/>
       <sheetName val="S1_TGS560_DIP"/>
       <sheetName val="LED_TGS560"/>
-      <sheetName val="X4_ACIN_4pin_TGS560_25"/>
-      <sheetName val="X1_DC_6pin_TGS560_25"/>
+      <sheetName val="X1_ACIN_4pin_TGS560_25"/>
+      <sheetName val="X4_DC_6pin_TGS560_25"/>
       <sheetName val="X5_RBR_3pin_TGS560_25"/>
       <sheetName val="X0a_48-100-xyz"/>
       <sheetName val="X0b_48-100-xyz"/>
@@ -15533,8 +15533,8 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18626,7 +18626,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added Acuro link to MIL versions FB1,2
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/connectors.en.xlsx
+++ b/docs/Manual/source/tab/connectors.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="50"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="48"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="583">
   <si>
     <t xml:space="preserve">This is a workbook with source tables of TGZ/TGS connector descriptions in English. Each sheet corresponds to one unique connector type. Since connectors are often repeated within TGZ (typically those on the control board), they are only listed once. I.e. E.g. IO connector 22pin weidmuller B2CF is used over and over again, so it is only listed here once as "X8_IO_22pin_B2CF"</t>
   </si>
@@ -1327,6 +1327,18 @@
     <t xml:space="preserve">RxD-</t>
   </si>
   <si>
+    <t xml:space="preserve">Hengstler Acuro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UB+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UB-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hengstler ACURO link</t>
+  </si>
+  <si>
     <t xml:space="preserve">AIN</t>
   </si>
   <si>
@@ -1828,37 +1840,37 @@
     <t xml:space="preserve">External P1000</t>
   </si>
   <si>
-    <t xml:space="preserve">EXC+</t>
+    <t xml:space="preserve">R2</t>
   </si>
   <si>
     <t xml:space="preserve">Resolver excitation +</t>
   </si>
   <si>
-    <t xml:space="preserve">EXC-</t>
+    <t xml:space="preserve">R1</t>
   </si>
   <si>
     <t xml:space="preserve">Resolver excitation -</t>
   </si>
   <si>
-    <t xml:space="preserve">SIN+</t>
+    <t xml:space="preserve">S1</t>
   </si>
   <si>
     <t xml:space="preserve">SIN + resolver output</t>
   </si>
   <si>
-    <t xml:space="preserve">SIN-</t>
+    <t xml:space="preserve">S3</t>
   </si>
   <si>
     <t xml:space="preserve">SIN - resolver output</t>
   </si>
   <si>
-    <t xml:space="preserve">COS+</t>
+    <t xml:space="preserve">S2</t>
   </si>
   <si>
     <t xml:space="preserve">COS + resolver output</t>
   </si>
   <si>
-    <t xml:space="preserve">COS-</t>
+    <t xml:space="preserve">S4</t>
   </si>
   <si>
     <t xml:space="preserve">COS - resolver output</t>
@@ -2165,6 +2177,7 @@
       <sheetName val="X5_FB1_10pin_ClikMate"/>
       <sheetName val="X6_FB2_10pin_ClikMate"/>
       <sheetName val="X7_AIN_12pin_ClikMate"/>
+      <sheetName val="X7_AIN_HALL_12pin_ClikMate"/>
       <sheetName val="X8_DIO_18pin_ClikMate"/>
       <sheetName val="X10_CAN_8pin_ClikMate"/>
       <sheetName val="X11_FB3_10pin_ClikMate"/>
@@ -3036,6 +3049,7 @@
       <sheetData sheetId="65"/>
       <sheetData sheetId="66"/>
       <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3155,7 +3169,7 @@
   <dimension ref="A1:L204"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I191" activeCellId="1" sqref="D1:D13 I191"/>
+      <selection pane="topLeft" activeCell="I191" activeCellId="1" sqref="F1 I191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9233,7 +9247,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="F1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9391,7 +9405,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9549,7 +9563,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D13 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="F1 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9679,7 +9693,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D13 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="F1 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9809,7 +9823,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="F1 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9922,7 +9936,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="D1:D13 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="F1 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9996,7 +10010,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D1:D13 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="F1 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10084,7 +10098,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10184,7 +10198,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="D1:D13 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="F1 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10272,7 +10286,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10374,7 +10388,7 @@
   <dimension ref="A1:H260"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="1" sqref="D1:D13 B52"/>
+      <selection pane="topLeft" activeCell="B52" activeCellId="1" sqref="F1 B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13505,7 +13519,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13607,7 +13621,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="D1:D13 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="F1 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13737,7 +13751,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13851,7 +13865,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="D1:D13 C6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="F1 C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13951,7 +13965,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14051,7 +14065,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14123,7 +14137,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="D1:D13 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="F1 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14253,7 +14267,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14439,7 +14453,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D13 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="F1 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14522,7 +14536,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14652,7 +14666,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D1:D13 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="F1 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14765,7 +14779,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="D1:D13 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="F1 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14976,7 +14990,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15077,7 +15091,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="F1 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15179,7 +15193,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="D1:D13 E32"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="F1 E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15281,7 +15295,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15383,7 +15397,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15485,7 +15499,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15568,7 +15582,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="D1:D13 C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="F1 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15735,7 +15749,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15835,7 +15849,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15935,7 +15949,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="D1:D13 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="F1 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16048,7 +16062,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="1" sqref="D1:D13 C18"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="1" sqref="F1 C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16207,7 +16221,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="D1:D13 C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="F1 C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16366,7 +16380,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O42" activeCellId="1" sqref="D1:D13 O42"/>
+      <selection pane="topLeft" activeCell="O42" activeCellId="1" sqref="F1 O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16461,7 +16475,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16574,7 +16588,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D1:D13 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="F1 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16706,7 +16720,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T15" activeCellId="1" sqref="D1:D13 T15"/>
+      <selection pane="topLeft" activeCell="T15" activeCellId="1" sqref="F1 T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16837,7 +16851,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="D1:D13 C19"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="F1 C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16968,7 +16982,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="1" sqref="D1:D13 E20"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="1" sqref="F1 E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17219,10 +17233,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="1" sqref="D1:D13 D20"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17249,6 +17263,9 @@
       <c r="E1" s="4" t="s">
         <v>390</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
@@ -17266,6 +17283,9 @@
       <c r="E2" s="4" t="s">
         <v>234</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
@@ -17283,6 +17303,9 @@
       <c r="E3" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -17300,6 +17323,9 @@
       <c r="E4" s="4" t="s">
         <v>392</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -17317,6 +17343,9 @@
       <c r="E5" s="4" t="s">
         <v>394</v>
       </c>
+      <c r="F5" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -17334,6 +17363,9 @@
       <c r="E6" s="4" t="s">
         <v>392</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -17351,6 +17383,9 @@
       <c r="E7" s="4" t="s">
         <v>394</v>
       </c>
+      <c r="F7" s="4" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
@@ -17368,6 +17403,9 @@
       <c r="E8" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
@@ -17385,6 +17423,9 @@
       <c r="E9" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="F9" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -17402,6 +17443,9 @@
       <c r="E10" s="4" t="s">
         <v>217</v>
       </c>
+      <c r="F10" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -17418,6 +17462,9 @@
       </c>
       <c r="E11" s="4" t="s">
         <v>151</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17439,10 +17486,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="1" sqref="D1:D13 J12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17469,6 +17516,9 @@
       <c r="E1" s="4" t="s">
         <v>390</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
@@ -17486,6 +17536,9 @@
       <c r="E2" s="4" t="s">
         <v>234</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
@@ -17503,6 +17556,9 @@
       <c r="E3" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -17520,6 +17576,9 @@
       <c r="E4" s="4" t="s">
         <v>392</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -17537,6 +17596,9 @@
       <c r="E5" s="4" t="s">
         <v>394</v>
       </c>
+      <c r="F5" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -17554,6 +17616,9 @@
       <c r="E6" s="4" t="s">
         <v>392</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -17571,6 +17636,9 @@
       <c r="E7" s="4" t="s">
         <v>394</v>
       </c>
+      <c r="F7" s="4" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
@@ -17588,6 +17656,9 @@
       <c r="E8" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
@@ -17605,6 +17676,9 @@
       <c r="E9" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="F9" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -17622,6 +17696,9 @@
       <c r="E10" s="4" t="s">
         <v>217</v>
       </c>
+      <c r="F10" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -17638,6 +17715,9 @@
       </c>
       <c r="E11" s="4" t="s">
         <v>151</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17662,7 +17742,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D13 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="F1 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17728,7 +17808,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17754,10 +17834,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17768,7 +17848,7 @@
         <v>159</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17776,10 +17856,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17787,10 +17867,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17798,10 +17878,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17809,10 +17889,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17820,10 +17900,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17834,7 +17914,7 @@
         <v>182</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17842,10 +17922,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17856,7 +17936,7 @@
         <v>182</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17864,10 +17944,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17878,7 +17958,7 @@
         <v>182</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17900,10 +17980,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="F1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17923,8 +18003,8 @@
       <c r="C1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>413</v>
+      <c r="D1" s="4" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17932,13 +18012,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>414</v>
+        <v>404</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17949,10 +18029,10 @@
         <v>159</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>415</v>
+        <v>405</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17960,13 +18040,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>416</v>
+        <v>407</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17974,13 +18054,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>415</v>
+        <v>407</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17988,13 +18068,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>416</v>
+        <v>410</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18002,13 +18082,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>415</v>
+        <v>410</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18016,13 +18096,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18030,13 +18110,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>415</v>
+        <v>425</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18044,13 +18124,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>423</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18058,13 +18138,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>419</v>
+        <v>429</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18072,13 +18152,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>419</v>
+        <v>431</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18086,41 +18166,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>419</v>
+        <v>433</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="12"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -18141,7 +18197,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="D1:D13 C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="F1 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18170,7 +18226,7 @@
         <v>198</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18181,7 +18237,7 @@
         <v>196</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18192,7 +18248,7 @@
         <v>194</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18203,7 +18259,7 @@
         <v>192</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18214,7 +18270,7 @@
         <v>190</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18225,7 +18281,7 @@
         <v>188</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18236,7 +18292,7 @@
         <v>186</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18247,7 +18303,7 @@
         <v>184</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18255,10 +18311,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18266,10 +18322,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18277,10 +18333,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18288,10 +18344,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18302,7 +18358,7 @@
         <v>176</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18313,7 +18369,7 @@
         <v>174</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18324,7 +18380,7 @@
         <v>172</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18335,7 +18391,7 @@
         <v>170</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18346,7 +18402,7 @@
         <v>168</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18357,7 +18413,7 @@
         <v>166</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -18379,7 +18435,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="D1:D13 C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="F1 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18405,10 +18461,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18416,10 +18472,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18427,10 +18483,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18438,10 +18494,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18449,10 +18505,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18460,10 +18516,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18471,10 +18527,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18482,10 +18538,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -18507,7 +18563,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="D1:D13 C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="F1 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18533,10 +18589,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18544,10 +18600,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18558,7 +18614,7 @@
         <v>398</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18569,7 +18625,7 @@
         <v>397</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18577,10 +18633,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18591,7 +18647,7 @@
         <v>151</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18599,10 +18655,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18610,10 +18666,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18624,7 +18680,7 @@
         <v>397</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18635,7 +18691,7 @@
         <v>398</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18666,7 +18722,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18692,10 +18748,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18703,10 +18759,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18714,10 +18770,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18725,10 +18781,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18736,10 +18792,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18747,10 +18803,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18758,10 +18814,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18769,10 +18825,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18809,7 +18865,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18841,10 +18897,10 @@
         <v>316</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18855,10 +18911,10 @@
         <v>314</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18872,7 +18928,7 @@
         <v>313</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18886,7 +18942,7 @@
         <v>307</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18900,7 +18956,7 @@
         <v>309</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18914,7 +18970,7 @@
         <v>311</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18925,10 +18981,10 @@
         <v>241</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18965,7 +19021,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18994,10 +19050,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>324</v>
@@ -19008,10 +19064,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>324</v>
@@ -19066,7 +19122,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="1" sqref="D1:D13 I24"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="1" sqref="F1 I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19096,13 +19152,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19110,13 +19166,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19127,10 +19183,10 @@
         <v>147</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19144,7 +19200,7 @@
         <v>153</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19158,7 +19214,7 @@
         <v>152</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -19180,7 +19236,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="D1:D13 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="F1 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19210,10 +19266,10 @@
         <v>155</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19224,10 +19280,10 @@
         <v>157</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19238,10 +19294,10 @@
         <v>241</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -19263,7 +19319,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19613,7 +19669,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="F1 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19645,10 +19701,10 @@
         <v>236</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19659,10 +19715,10 @@
         <v>239</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19676,7 +19732,7 @@
         <v>242</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19690,7 +19746,7 @@
         <v>244</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19704,7 +19760,7 @@
         <v>246</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19718,7 +19774,7 @@
         <v>248</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19743,7 +19799,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19775,10 +19831,10 @@
         <v>236</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19789,10 +19845,10 @@
         <v>239</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19806,7 +19862,7 @@
         <v>242</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19820,7 +19876,7 @@
         <v>244</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19834,7 +19890,7 @@
         <v>246</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19848,7 +19904,7 @@
         <v>248</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19873,7 +19929,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="D1:D13 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="F1 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19889,7 +19945,7 @@
         <v>377</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>141</v>
@@ -19897,162 +19953,162 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
+        <v>530</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>526</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>522</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="C18" s="12"/>
       <c r="H18" s="4"/>
@@ -20060,50 +20116,50 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="15"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="15"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="15"/>
@@ -20127,7 +20183,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="D1:D13 D18"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="F1 D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20140,10 +20196,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>141</v>
@@ -20151,107 +20207,107 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="15"/>
@@ -20263,7 +20319,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>141</v>
@@ -20273,20 +20329,20 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="15"/>
@@ -20342,7 +20398,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20374,10 +20430,10 @@
         <v>241</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20391,7 +20447,7 @@
         <v>307</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20405,7 +20461,7 @@
         <v>309</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20419,7 +20475,7 @@
         <v>311</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20456,7 +20512,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20488,10 +20544,10 @@
         <v>155</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20502,10 +20558,10 @@
         <v>157</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20516,10 +20572,10 @@
         <v>241</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20530,10 +20586,10 @@
         <v>155</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20544,10 +20600,10 @@
         <v>157</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20558,10 +20614,10 @@
         <v>241</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20601,7 +20657,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="D1:D13 E34"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="F1 E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20636,7 +20692,7 @@
         <v>313</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20647,10 +20703,10 @@
         <v>314</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20661,10 +20717,10 @@
         <v>316</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20704,7 +20760,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="D1:D13 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="F1 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20734,10 +20790,10 @@
         <v>243</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20748,10 +20804,10 @@
         <v>245</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20762,10 +20818,10 @@
         <v>247</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20779,7 +20835,7 @@
         <v>156</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20793,7 +20849,7 @@
         <v>251</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -20815,7 +20871,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="F1 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20845,10 +20901,10 @@
         <v>151</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20856,13 +20912,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20873,10 +20929,10 @@
         <v>230</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20887,10 +20943,10 @@
         <v>232</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>563</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20901,10 +20957,10 @@
         <v>151</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20918,7 +20974,7 @@
         <v>148</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20932,7 +20988,7 @@
         <v>144</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20946,7 +21002,7 @@
         <v>146</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20957,10 +21013,10 @@
         <v>320</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20971,10 +21027,10 @@
         <v>318</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21032,7 +21088,7 @@
   <dimension ref="A1:C1009"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="D1:D13 C15"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="1" sqref="F1 J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21058,10 +21114,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21069,10 +21125,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21080,10 +21136,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21091,10 +21147,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21102,10 +21158,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21113,10 +21169,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21127,7 +21183,7 @@
         <v>159</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21138,7 +21194,7 @@
         <v>159</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24164,7 +24220,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="D1:D13 C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="F1 C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24262,7 +24318,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="D1:D13 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="F1 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24313,7 +24369,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D13"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="F1 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
added hand crimping tool notes, added X1 S-100/XYZ CZ version detailed connector desc.
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/connectors.en.xlsx
+++ b/docs/Manual/source/tab/connectors.en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="48"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -964,13 +964,13 @@
     <t xml:space="preserve">+24V DC Brake power</t>
   </si>
   <si>
+    <t xml:space="preserve">+ Static brake</t>
+  </si>
+  <si>
     <t xml:space="preserve">VCCD</t>
   </si>
   <si>
     <t xml:space="preserve">+24V DC Brake diag. power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+ Static brake</t>
   </si>
   <si>
     <t xml:space="preserve">- Static brake</t>
@@ -3169,7 +3169,7 @@
   <dimension ref="A1:L204"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I191" activeCellId="1" sqref="F1 I191"/>
+      <selection pane="topLeft" activeCell="I191" activeCellId="1" sqref="B4:C4 I191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9247,7 +9247,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="F1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B4:C4 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9405,7 +9405,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9563,7 +9563,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="F1 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B4:C4 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9693,7 +9693,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="F1 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B4:C4 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9823,7 +9823,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="F1 D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="B4:C4 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9936,7 +9936,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="F1 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="B4:C4 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10010,7 +10010,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="F1 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B4:C4 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10098,7 +10098,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10198,7 +10198,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="F1 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10286,7 +10286,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10388,7 +10388,7 @@
   <dimension ref="A1:H260"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="1" sqref="F1 B52"/>
+      <selection pane="topLeft" activeCell="B52" activeCellId="1" sqref="B4:C4 B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13519,7 +13519,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13621,7 +13621,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="F1 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="B4:C4 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13751,7 +13751,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13862,10 +13862,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="F1 C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13909,10 +13909,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>279</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>274</v>
@@ -13923,7 +13923,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>280</v>
@@ -13945,6 +13945,10 @@
       <c r="D5" s="4" t="s">
         <v>274</v>
       </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -13965,7 +13969,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14065,7 +14069,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14137,7 +14141,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="F1 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="B4:C4 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14267,7 +14271,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14453,7 +14457,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="F1 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B4:C4 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14536,7 +14540,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14666,7 +14670,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="F1 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B4:C4 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14779,7 +14783,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="F1 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="B4:C4 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14990,7 +14994,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15091,7 +15095,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="F1 D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="B4:C4 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15193,7 +15197,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="F1 E32"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="B4:C4 E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15295,7 +15299,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15397,7 +15401,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15499,7 +15503,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15582,7 +15586,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="F1 C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="B4:C4 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15749,7 +15753,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15849,7 +15853,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15949,7 +15953,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="F1 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="B4:C4 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16062,7 +16066,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="1" sqref="F1 C18"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="1" sqref="B4:C4 C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16221,7 +16225,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="F1 C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="B4:C4 C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16380,7 +16384,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O42" activeCellId="1" sqref="F1 O42"/>
+      <selection pane="topLeft" activeCell="O42" activeCellId="1" sqref="B4:C4 O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16475,7 +16479,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16588,7 +16592,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="F1 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B4:C4 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16720,7 +16724,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T15" activeCellId="1" sqref="F1 T15"/>
+      <selection pane="topLeft" activeCell="T15" activeCellId="1" sqref="B4:C4 T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16851,7 +16855,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="F1 C19"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="B4:C4 C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16982,7 +16986,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="1" sqref="F1 E20"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="1" sqref="B4:C4 E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17236,7 +17240,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="B4:C4 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17488,8 +17492,8 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="B4:C4 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17742,7 +17746,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="F1 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B4:C4 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17808,7 +17812,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17983,7 +17987,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="F1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B4:C4 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18197,7 +18201,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="F1 C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="B4:C4 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18435,7 +18439,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="F1 C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="B4:C4 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18563,7 +18567,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="F1 C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="B4:C4 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18722,7 +18726,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18865,7 +18869,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19021,7 +19025,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19122,7 +19126,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="1" sqref="F1 I24"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="1" sqref="B4:C4 I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19236,7 +19240,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="F1 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19319,7 +19323,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19669,7 +19673,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="F1 D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="B4:C4 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19799,7 +19803,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19929,7 +19933,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="F1 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20183,7 +20187,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="F1 D18"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="B4:C4 D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20398,7 +20402,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20512,7 +20516,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20657,7 +20661,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="F1 E34"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="B4:C4 E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20760,7 +20764,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="F1 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="B4:C4 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20871,7 +20875,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="F1 D8"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="B4:C4 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21088,7 +21092,7 @@
   <dimension ref="A1:C1009"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="1" sqref="F1 J9"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="1" sqref="B4:C4 J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24220,7 +24224,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="F1 C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="B4:C4 C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24318,7 +24322,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="F1 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="B4:C4 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24369,7 +24373,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="F1 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B4:C4 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>